<commit_message>
2nd commit of the day
</commit_message>
<xml_diff>
--- a/com.ecommerce.automation/src/main/java/com/ecommerce/xls/Login functionality.xlsx
+++ b/com.ecommerce.automation/src/main/java/com/ecommerce/xls/Login functionality.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="3480" windowWidth="10545" xWindow="0" yWindow="2520"/>
+    <workbookView activeTab="1" windowHeight="3480" windowWidth="10545" xWindow="0" yWindow="2520"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" r:id="rId1" sheetId="1"/>
@@ -14,11 +14,12 @@
     <sheet name="ResetPassword" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="C33:F42"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="109">
   <si>
     <t>TCID</t>
   </si>
@@ -320,6 +321,15 @@
     <t>Result9</t>
   </si>
   <si>
+    <t>loginEmail_css</t>
+  </si>
+  <si>
+    <t>loginPassword_css</t>
+  </si>
+  <si>
+    <t>loginButton_css</t>
+  </si>
+  <si>
     <t>Note</t>
   </si>
   <si>
@@ -335,10 +345,7 @@
     <t>resetEmailAddress_css</t>
   </si>
   <si>
-    <t>clickLink_xpath</t>
-  </si>
-  <si>
-    <t>LoginLink_xpath</t>
+    <t>Result10</t>
   </si>
 </sst>
 </file>
@@ -364,7 +371,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="31">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,6 +543,11 @@
         <fgColor indexed="55"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -692,9 +704,7 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="4" fillId="18" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="10" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf applyFill="true" borderId="0" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -994,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1020,7 +1030,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1046,7 +1056,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1072,7 +1082,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1086,7 +1096,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1112,7 +1122,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1135,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1150,8 +1160,17 @@
     <col min="5" max="5" customWidth="true" style="2" width="24.7109375" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="2" width="21.140625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
-    <col min="8" max="16" bestFit="true" customWidth="true" style="2" width="7.7109375" collapsed="true"/>
-    <col min="17" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.69921875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.69921875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.69921875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.69921875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.69921875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.69921875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.69921875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.69921875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.8125" collapsed="true"/>
+    <col min="18" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -1202,6 +1221,9 @@
       </c>
       <c r="P1" s="45" t="s">
         <v>99</v>
+      </c>
+      <c r="Q1" s="50" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1664,7 +1686,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:7">
       <c r="A17" s="12" t="s">
         <v>31</v>
       </c>
@@ -1675,7 +1697,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:7">
       <c r="A18" s="12" t="s">
         <v>31</v>
       </c>
@@ -1686,7 +1708,7 @@
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:7">
       <c r="A19" s="12" t="s">
         <v>31</v>
       </c>
@@ -1697,7 +1719,7 @@
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:7">
       <c r="A20" s="47"/>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
@@ -1706,7 +1728,7 @@
       <c r="F20" s="48"/>
       <c r="G20" s="49"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:7">
       <c r="A21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1721,7 +1743,7 @@
       </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:7">
       <c r="A22" s="10" t="s">
         <v>52</v>
       </c>
@@ -1736,7 +1758,7 @@
       </c>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:7">
       <c r="A23" s="10" t="s">
         <v>52</v>
       </c>
@@ -1753,7 +1775,7 @@
       </c>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:7">
       <c r="A24" s="10" t="s">
         <v>52</v>
       </c>
@@ -1770,7 +1792,7 @@
       </c>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:7">
       <c r="A25" s="10" t="s">
         <v>52</v>
       </c>
@@ -1785,7 +1807,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:7">
       <c r="A26" s="47"/>
       <c r="B26" s="48"/>
       <c r="C26" s="48"/>
@@ -1794,7 +1816,7 @@
       <c r="F26" s="48"/>
       <c r="G26" s="49"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:7">
       <c r="A27" s="18" t="s">
         <v>19</v>
       </c>
@@ -1808,9 +1830,6 @@
         <v>10</v>
       </c>
       <c r="G27" s="18"/>
-      <c r="H27" t="s">
-        <v>70</v>
-      </c>
       <c r="I27" t="s">
         <v>71</v>
       </c>
@@ -1836,7 +1855,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:7">
       <c r="A28" s="18" t="s">
         <v>19</v>
       </c>
@@ -1850,9 +1869,6 @@
         <v>12</v>
       </c>
       <c r="G28" s="18"/>
-      <c r="H28" t="s">
-        <v>70</v>
-      </c>
       <c r="I28" t="s">
         <v>71</v>
       </c>
@@ -1878,23 +1894,22 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:7">
       <c r="A29" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="F29" s="18"/>
+        <v>100</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="G29" s="18"/>
-      <c r="H29" t="s">
-        <v>70</v>
-      </c>
       <c r="I29" t="s">
         <v>71</v>
       </c>
@@ -1920,23 +1935,22 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:7">
       <c r="A30" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
       <c r="D30" s="18" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="18"/>
+        <v>101</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>46</v>
+      </c>
       <c r="G30" s="18"/>
-      <c r="H30" t="s">
-        <v>70</v>
-      </c>
       <c r="I30" t="s">
         <v>71</v>
       </c>
@@ -1962,16 +1976,18 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:7">
       <c r="A31" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E31" s="18"/>
+        <v>76</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>102</v>
+      </c>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="I31" t="s">
@@ -1999,44 +2015,90 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="47"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="49"/>
+    <row r="32" spans="1:7">
+      <c r="A32" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="I32" t="s">
+        <v>71</v>
+      </c>
+      <c r="J32" t="s">
+        <v>71</v>
+      </c>
+      <c r="K32" t="s">
+        <v>71</v>
+      </c>
+      <c r="L32" t="s">
+        <v>71</v>
+      </c>
+      <c r="M32" t="s">
+        <v>71</v>
+      </c>
+      <c r="N32" t="s">
+        <v>71</v>
+      </c>
+      <c r="O32" t="s">
+        <v>71</v>
+      </c>
+      <c r="P32" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="13"/>
+      <c r="A33" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="I33" t="s">
+        <v>71</v>
+      </c>
+      <c r="J33" t="s">
+        <v>71</v>
+      </c>
+      <c r="K33" t="s">
+        <v>71</v>
+      </c>
+      <c r="L33" t="s">
+        <v>71</v>
+      </c>
+      <c r="M33" t="s">
+        <v>71</v>
+      </c>
+      <c r="N33" t="s">
+        <v>71</v>
+      </c>
+      <c r="O33" t="s">
+        <v>71</v>
+      </c>
+      <c r="P33" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="13"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="49"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="13" t="s">
@@ -2045,13 +2107,11 @@
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>14</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E35" s="13"/>
       <c r="F35" s="13" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="G35" s="13"/>
     </row>
@@ -2062,13 +2122,11 @@
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>15</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E36" s="13"/>
       <c r="F36" s="13" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="G36" s="13"/>
     </row>
@@ -2079,12 +2137,14 @@
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" s="13"/>
+        <v>14</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="G37" s="13"/>
     </row>
     <row r="38" spans="1:7">
@@ -2094,12 +2154,14 @@
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F38" s="13"/>
+        <v>15</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="G38" s="13"/>
     </row>
     <row r="39" spans="1:7">
@@ -2108,49 +2170,49 @@
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="13"/>
+      <c r="D39" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="47"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="49"/>
+      <c r="A40" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" s="9"/>
+      <c r="A41" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="9"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="49"/>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="9" t="s">
@@ -2159,13 +2221,11 @@
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>14</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E43" s="9"/>
       <c r="F43" s="9" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="G43" s="9"/>
     </row>
@@ -2176,13 +2236,11 @@
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>15</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E44" s="9"/>
       <c r="F44" s="9" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="G44" s="9"/>
     </row>
@@ -2193,12 +2251,14 @@
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F45" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7">
@@ -2208,50 +2268,52 @@
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="9"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="47"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="49"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G49" s="8"/>
+      <c r="A49" s="47"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="49"/>
     </row>
     <row r="50" spans="1:16">
       <c r="A50" s="8" t="s">
@@ -2260,13 +2322,11 @@
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>14</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E50" s="8"/>
       <c r="F50" s="8" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="G50" s="8"/>
     </row>
@@ -2277,13 +2337,11 @@
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>15</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E51" s="8"/>
       <c r="F51" s="8" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="G51" s="8"/>
     </row>
@@ -2294,12 +2352,14 @@
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F52" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:16">
@@ -2309,12 +2369,14 @@
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F53" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="G53" s="8"/>
     </row>
     <row r="54" spans="1:16">
@@ -2323,8 +2385,12 @@
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="D54" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
     </row>
@@ -2334,8 +2400,12 @@
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
+      <c r="D55" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
     </row>
@@ -2351,128 +2421,35 @@
       <c r="G56" s="8"/>
     </row>
     <row r="57" spans="1:16">
-      <c r="A57" s="47"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="49"/>
-      <c r="H57" t="s">
-        <v>70</v>
-      </c>
-      <c r="I57" t="s">
-        <v>71</v>
-      </c>
-      <c r="J57" t="s">
-        <v>71</v>
-      </c>
-      <c r="K57" t="s">
-        <v>71</v>
-      </c>
-      <c r="L57" t="s">
-        <v>71</v>
-      </c>
-      <c r="M57" t="s">
-        <v>71</v>
-      </c>
-      <c r="N57" t="s">
-        <v>71</v>
-      </c>
-      <c r="O57" t="s">
-        <v>71</v>
-      </c>
-      <c r="P57" t="s">
-        <v>71</v>
-      </c>
+      <c r="A57" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:16">
-      <c r="A58" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G58" s="12"/>
-      <c r="H58" t="s">
-        <v>70</v>
-      </c>
-      <c r="I58" t="s">
-        <v>71</v>
-      </c>
-      <c r="J58" t="s">
-        <v>71</v>
-      </c>
-      <c r="K58" t="s">
-        <v>71</v>
-      </c>
-      <c r="L58" t="s">
-        <v>71</v>
-      </c>
-      <c r="M58" t="s">
-        <v>71</v>
-      </c>
-      <c r="N58" t="s">
-        <v>71</v>
-      </c>
-      <c r="O58" t="s">
-        <v>71</v>
-      </c>
-      <c r="P58" t="s">
-        <v>71</v>
-      </c>
+      <c r="A58" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="12"/>
-      <c r="H59" t="s">
-        <v>70</v>
-      </c>
-      <c r="I59" t="s">
-        <v>71</v>
-      </c>
-      <c r="J59" t="s">
-        <v>71</v>
-      </c>
-      <c r="K59" t="s">
-        <v>71</v>
-      </c>
-      <c r="L59" t="s">
-        <v>71</v>
-      </c>
-      <c r="M59" t="s">
-        <v>71</v>
-      </c>
-      <c r="N59" t="s">
-        <v>71</v>
-      </c>
-      <c r="O59" t="s">
-        <v>71</v>
-      </c>
-      <c r="P59" t="s">
-        <v>71</v>
-      </c>
+      <c r="A59" s="47"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="48"/>
+      <c r="E59" s="48"/>
+      <c r="F59" s="48"/>
+      <c r="G59" s="49"/>
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="12" t="s">
@@ -2480,15 +2457,15 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="F60" s="12"/>
+        <v>9</v>
+      </c>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="G60" s="12"/>
       <c r="H60" t="s">
         <v>70</v>
@@ -2517,6 +2494,9 @@
       <c r="P60" t="s">
         <v>71</v>
       </c>
+      <c r="Q60" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="61" spans="1:16">
       <c r="A61" s="12" t="s">
@@ -2524,16 +2504,14 @@
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>104</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E61" s="12"/>
       <c r="F61" s="12" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G61" s="12"/>
       <c r="H61" t="s">
@@ -2563,6 +2541,9 @@
       <c r="P61" t="s">
         <v>71</v>
       </c>
+      <c r="Q61" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="12" t="s">
@@ -2570,13 +2551,13 @@
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
@@ -2607,20 +2588,27 @@
       <c r="P62" t="s">
         <v>71</v>
       </c>
+      <c r="Q62" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
+      <c r="C63" s="12" t="s">
+        <v>66</v>
+      </c>
       <c r="D63" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E63" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="F63" s="12"/>
+        <v>75</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>45</v>
+      </c>
       <c r="G63" s="12"/>
       <c r="H63" t="s">
         <v>70</v>
@@ -2649,39 +2637,164 @@
       <c r="P63" t="s">
         <v>71</v>
       </c>
+      <c r="Q63" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="64" spans="1:16">
       <c r="A64" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
+      <c r="C64" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="D64" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E64" s="12"/>
+        <v>76</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="47"/>
-      <c r="B65" s="48"/>
-      <c r="C65" s="48"/>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="48"/>
-      <c r="G65" s="49"/>
+      <c r="H64" t="s">
+        <v>70</v>
+      </c>
+      <c r="I64" t="s">
+        <v>71</v>
+      </c>
+      <c r="J64" t="s">
+        <v>71</v>
+      </c>
+      <c r="K64" t="s">
+        <v>71</v>
+      </c>
+      <c r="L64" t="s">
+        <v>71</v>
+      </c>
+      <c r="M64" t="s">
+        <v>71</v>
+      </c>
+      <c r="N64" t="s">
+        <v>71</v>
+      </c>
+      <c r="O64" t="s">
+        <v>71</v>
+      </c>
+      <c r="P64" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="A65" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E65" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" t="s">
+        <v>70</v>
+      </c>
+      <c r="I65" t="s">
+        <v>71</v>
+      </c>
+      <c r="J65" t="s">
+        <v>71</v>
+      </c>
+      <c r="K65" t="s">
+        <v>71</v>
+      </c>
+      <c r="L65" t="s">
+        <v>71</v>
+      </c>
+      <c r="M65" t="s">
+        <v>71</v>
+      </c>
+      <c r="N65" t="s">
+        <v>71</v>
+      </c>
+      <c r="O65" t="s">
+        <v>71</v>
+      </c>
+      <c r="P65" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
+      <c r="A66" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" t="s">
+        <v>70</v>
+      </c>
+      <c r="I66" t="s">
+        <v>71</v>
+      </c>
+      <c r="J66" t="s">
+        <v>71</v>
+      </c>
+      <c r="K66" t="s">
+        <v>71</v>
+      </c>
+      <c r="L66" t="s">
+        <v>71</v>
+      </c>
+      <c r="M66" t="s">
+        <v>71</v>
+      </c>
+      <c r="N66" t="s">
+        <v>71</v>
+      </c>
+      <c r="O66" t="s">
+        <v>71</v>
+      </c>
+      <c r="P66" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
+      <c r="A67" s="47"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="48"/>
+      <c r="D67" s="48"/>
+      <c r="E67" s="48"/>
+      <c r="F67" s="48"/>
+      <c r="G67" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="A67:G67"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A20:G20"/>
     <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A47:G47"/>
-    <mergeCell ref="A57:G57"/>
-    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="A59:G59"/>
+    <mergeCell ref="A34:G34"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2690,7 +2803,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
@@ -2909,10 +3022,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2951,7 +3064,7 @@
         <v>8123204729</v>
       </c>
       <c r="B2" s="21">
-        <v>8123204729</v>
+        <v>81232047</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2963,26 +3076,141 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="24">
-        <v>8123204729</v>
-      </c>
-      <c r="B3" s="24">
-        <v>8123204729</v>
+      <c r="A3" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>41</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
-      <c r="E3" s="50" t="s">
-        <v>40</v>
+      <c r="E3" s="26" t="s">
+        <v>3</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink display="pass@1234" r:id="rId1" ref="B2"/>
     <hyperlink display="sayem4@gmail.com" r:id="rId2" ref="A3"/>
-    <hyperlink display="sayem4@gmail.com" r:id="rId3" ref="A2"/>
+    <hyperlink display="pass@1234" r:id="rId3" ref="B3"/>
+    <hyperlink display="sayem4@gmail.com" r:id="rId4" ref="A5"/>
+    <hyperlink display="sayem4@gmail.com" r:id="rId5" ref="A2"/>
+    <hyperlink display="pass@1234" r:id="rId6" ref="B6"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2990,7 +3218,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
@@ -3000,7 +3228,7 @@
   <cols>
     <col min="1" max="1" customWidth="true" style="20" width="25.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="20" width="10.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="20" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="20" width="6.58203125" collapsed="true"/>
     <col min="4" max="16384" style="20" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
@@ -3111,6 +3339,11 @@
         <v>3</v>
       </c>
       <c r="C10" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>